<commit_message>
correcao da ultima atividade ("outras") - sem categoria, só duração
</commit_message>
<xml_diff>
--- a/others/activitiesClassification.xlsx
+++ b/others/activitiesClassification.xlsx
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="car" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="123">
   <si>
     <t>Cycling, sport</t>
   </si>
@@ -391,7 +391,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -523,6 +523,14 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -878,7 +886,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -888,12 +896,6 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -906,6 +908,15 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1251,8 +1262,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="I61" sqref="I61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1264,55 +1275,55 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
     </row>
     <row r="2" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="9"/>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="4" t="s">
+      <c r="A2" s="7"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="3" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="7">
+      <c r="A3" s="5">
         <v>-1</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="5" t="s">
         <v>64</v>
       </c>
       <c r="D3" s="1" t="s">
@@ -1323,13 +1334,13 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="7">
+      <c r="A4" s="5">
         <v>-1</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="5" t="s">
         <v>68</v>
       </c>
       <c r="D4" s="1" t="s">
@@ -1340,13 +1351,13 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="7">
+      <c r="A5" s="5">
         <v>-1</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="5" t="s">
         <v>7</v>
       </c>
       <c r="D5" s="1" t="s">
@@ -1357,13 +1368,13 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="7">
+      <c r="A6" s="5">
         <v>-1</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="5" t="s">
         <v>119</v>
       </c>
       <c r="D6" s="1" t="s">
@@ -1374,13 +1385,13 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="7">
+      <c r="A7" s="5">
         <v>-1</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="5" t="s">
         <v>81</v>
       </c>
       <c r="D7" s="1" t="s">
@@ -1391,13 +1402,13 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="7">
+      <c r="A8" s="5">
         <v>-1</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="5" t="s">
         <v>25</v>
       </c>
       <c r="D8" s="1" t="s">
@@ -1408,13 +1419,13 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="7">
+      <c r="A9" s="5">
         <v>-1</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="5" t="s">
         <v>86</v>
       </c>
       <c r="D9" s="1" t="s">
@@ -1425,13 +1436,13 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="7">
+      <c r="A10" s="5">
         <v>-1</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="5" t="s">
         <v>29</v>
       </c>
       <c r="D10" s="1" t="s">
@@ -1442,13 +1453,13 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="7">
+      <c r="A11" s="5">
         <v>-1</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="5" t="s">
         <v>87</v>
       </c>
       <c r="D11" s="1" t="s">
@@ -1459,13 +1470,13 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="7">
+      <c r="A12" s="5">
         <v>-1</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C12" s="5" t="s">
         <v>90</v>
       </c>
       <c r="D12" s="1" t="s">
@@ -1476,13 +1487,13 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="7">
+      <c r="A13" s="5">
         <v>-1</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="5" t="s">
         <v>100</v>
       </c>
       <c r="D13" s="1" t="s">
@@ -1493,13 +1504,13 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="7">
+      <c r="A14" s="5">
         <v>-1</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C14" s="5" t="s">
         <v>104</v>
       </c>
       <c r="D14" s="1" t="s">
@@ -1510,13 +1521,13 @@
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="7">
+      <c r="A15" s="5">
         <v>-1</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="C15" s="5" t="s">
         <v>105</v>
       </c>
       <c r="D15" s="1" t="s">
@@ -1527,13 +1538,13 @@
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="7">
+      <c r="A16" s="5">
         <v>-1</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="B16" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="C16" s="5" t="s">
         <v>106</v>
       </c>
       <c r="D16" s="1" t="s">
@@ -1544,13 +1555,13 @@
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="7">
+      <c r="A17" s="5">
         <v>-1</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="B17" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="C17" s="5" t="s">
         <v>107</v>
       </c>
       <c r="D17" s="1" t="s">
@@ -1561,13 +1572,13 @@
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="7">
+      <c r="A18" s="5">
         <v>-1</v>
       </c>
-      <c r="B18" s="7" t="s">
+      <c r="B18" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C18" s="7" t="s">
+      <c r="C18" s="5" t="s">
         <v>109</v>
       </c>
       <c r="D18" s="1" t="s">
@@ -1578,13 +1589,13 @@
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="7">
+      <c r="A19" s="5">
         <v>-1</v>
       </c>
-      <c r="B19" s="7" t="s">
+      <c r="B19" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="C19" s="7" t="s">
+      <c r="C19" s="5" t="s">
         <v>110</v>
       </c>
       <c r="D19" s="1" t="s">
@@ -1595,13 +1606,13 @@
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="8">
+      <c r="A20" s="6">
         <v>-1</v>
       </c>
-      <c r="B20" s="8" t="s">
+      <c r="B20" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="C20" s="8" t="s">
+      <c r="C20" s="6" t="s">
         <v>112</v>
       </c>
       <c r="D20" s="2" t="s">
@@ -1616,13 +1627,13 @@
       <c r="I20" s="2"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="7">
+      <c r="A21" s="5">
         <v>0</v>
       </c>
-      <c r="B21" s="7" t="s">
+      <c r="B21" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C21" s="7" t="s">
+      <c r="C21" s="5" t="s">
         <v>70</v>
       </c>
       <c r="E21" s="1" t="s">
@@ -1630,14 +1641,14 @@
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="7">
+      <c r="A22" s="5">
         <f>A21+1</f>
         <v>1</v>
       </c>
-      <c r="B22" s="7" t="s">
+      <c r="B22" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C22" s="7" t="s">
+      <c r="C22" s="5" t="s">
         <v>73</v>
       </c>
       <c r="E22" s="1" t="s">
@@ -1645,14 +1656,14 @@
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="7">
+      <c r="A23" s="5">
         <f t="shared" ref="A23:A62" si="0">A22+1</f>
         <v>2</v>
       </c>
-      <c r="B23" s="7" t="s">
+      <c r="B23" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C23" s="7" t="s">
+      <c r="C23" s="5" t="s">
         <v>74</v>
       </c>
       <c r="E23" s="1" t="s">
@@ -1660,14 +1671,14 @@
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="7">
+      <c r="A24" s="5">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="B24" s="7" t="s">
+      <c r="B24" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="7" t="s">
+      <c r="C24" s="5" t="s">
         <v>21</v>
       </c>
       <c r="E24" s="1" t="s">
@@ -1675,14 +1686,14 @@
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="7">
+      <c r="A25" s="5">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B25" s="7" t="s">
+      <c r="B25" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C25" s="7" t="s">
+      <c r="C25" s="5" t="s">
         <v>75</v>
       </c>
       <c r="E25" s="1" t="s">
@@ -1690,14 +1701,14 @@
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="7">
+      <c r="A26" s="5">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B26" s="7" t="s">
+      <c r="B26" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C26" s="7" t="s">
+      <c r="C26" s="5" t="s">
         <v>113</v>
       </c>
       <c r="E26" s="1" t="s">
@@ -1705,14 +1716,14 @@
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="7">
+      <c r="A27" s="5">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B27" s="7" t="s">
+      <c r="B27" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C27" s="7" t="s">
+      <c r="C27" s="5" t="s">
         <v>80</v>
       </c>
       <c r="E27" s="1" t="s">
@@ -1720,14 +1731,14 @@
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="7">
+      <c r="A28" s="5">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B28" s="7" t="s">
+      <c r="B28" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C28" s="7" t="s">
+      <c r="C28" s="5" t="s">
         <v>72</v>
       </c>
       <c r="E28" s="1" t="s">
@@ -1735,14 +1746,14 @@
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="7">
+      <c r="A29" s="5">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B29" s="7" t="s">
+      <c r="B29" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C29" s="7" t="s">
+      <c r="C29" s="5" t="s">
         <v>63</v>
       </c>
       <c r="F29" s="1" t="s">
@@ -1750,14 +1761,14 @@
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="7">
+      <c r="A30" s="5">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="B30" s="7" t="s">
+      <c r="B30" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C30" s="7" t="s">
+      <c r="C30" s="5" t="s">
         <v>65</v>
       </c>
       <c r="F30" s="1" t="s">
@@ -1765,14 +1776,14 @@
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="7">
+      <c r="A31" s="5">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="B31" s="7" t="s">
+      <c r="B31" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C31" s="7" t="s">
+      <c r="C31" s="5" t="s">
         <v>66</v>
       </c>
       <c r="F31" s="1" t="s">
@@ -1780,14 +1791,14 @@
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="7">
+      <c r="A32" s="5">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="B32" s="7" t="s">
+      <c r="B32" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C32" s="7" t="s">
+      <c r="C32" s="5" t="s">
         <v>69</v>
       </c>
       <c r="F32" s="1" t="s">
@@ -1795,14 +1806,14 @@
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="7">
+      <c r="A33" s="5">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="B33" s="7" t="s">
+      <c r="B33" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C33" s="7" t="s">
+      <c r="C33" s="5" t="s">
         <v>77</v>
       </c>
       <c r="F33" s="1" t="s">
@@ -1810,14 +1821,14 @@
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="7">
+      <c r="A34" s="5">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="B34" s="7" t="s">
+      <c r="B34" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C34" s="7" t="s">
+      <c r="C34" s="5" t="s">
         <v>67</v>
       </c>
       <c r="G34" s="1" t="s">
@@ -1825,14 +1836,14 @@
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="7">
+      <c r="A35" s="5">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="B35" s="7" t="s">
+      <c r="B35" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C35" s="7" t="s">
+      <c r="C35" s="5" t="s">
         <v>71</v>
       </c>
       <c r="G35" s="1" t="s">
@@ -1840,14 +1851,14 @@
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="7">
+      <c r="A36" s="5">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="B36" s="7" t="s">
+      <c r="B36" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C36" s="7" t="s">
+      <c r="C36" s="5" t="s">
         <v>76</v>
       </c>
       <c r="G36" s="1" t="s">
@@ -1855,14 +1866,14 @@
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="7">
+      <c r="A37" s="5">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="B37" s="7" t="s">
+      <c r="B37" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C37" s="7" t="s">
+      <c r="C37" s="5" t="s">
         <v>79</v>
       </c>
       <c r="G37" s="1" t="s">
@@ -1870,14 +1881,14 @@
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="7">
+      <c r="A38" s="5">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="B38" s="7" t="s">
+      <c r="B38" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C38" s="7" t="s">
+      <c r="C38" s="5" t="s">
         <v>103</v>
       </c>
       <c r="G38" s="1" t="s">
@@ -1885,14 +1896,14 @@
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" s="7">
+      <c r="A39" s="5">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="B39" s="7" t="s">
+      <c r="B39" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="C39" s="7" t="s">
+      <c r="C39" s="5" t="s">
         <v>108</v>
       </c>
       <c r="G39" s="1" t="s">
@@ -1900,14 +1911,14 @@
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" s="7">
+      <c r="A40" s="5">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="B40" s="7" t="s">
+      <c r="B40" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C40" s="7" t="s">
+      <c r="C40" s="5" t="s">
         <v>83</v>
       </c>
       <c r="H40" s="1" t="s">
@@ -1915,14 +1926,14 @@
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" s="7">
+      <c r="A41" s="5">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="B41" s="7" t="s">
+      <c r="B41" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C41" s="7" t="s">
+      <c r="C41" s="5" t="s">
         <v>88</v>
       </c>
       <c r="H41" s="1" t="s">
@@ -1930,14 +1941,14 @@
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" s="7">
+      <c r="A42" s="5">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="B42" s="7" t="s">
+      <c r="B42" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C42" s="7" t="s">
+      <c r="C42" s="5" t="s">
         <v>40</v>
       </c>
       <c r="H42" s="1" t="s">
@@ -1945,14 +1956,14 @@
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A43" s="7">
+      <c r="A43" s="5">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="B43" s="7" t="s">
+      <c r="B43" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C43" s="7" t="s">
+      <c r="C43" s="5" t="s">
         <v>95</v>
       </c>
       <c r="H43" s="1" t="s">
@@ -1960,14 +1971,14 @@
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A44" s="7">
+      <c r="A44" s="5">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="B44" s="7" t="s">
+      <c r="B44" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="C44" s="7" t="s">
+      <c r="C44" s="5" t="s">
         <v>101</v>
       </c>
       <c r="H44" s="1" t="s">
@@ -1975,14 +1986,14 @@
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A45" s="7">
+      <c r="A45" s="5">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="B45" s="7" t="s">
+      <c r="B45" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="C45" s="7" t="s">
+      <c r="C45" s="5" t="s">
         <v>120</v>
       </c>
       <c r="H45" s="1" t="s">
@@ -1990,14 +2001,14 @@
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A46" s="7">
+      <c r="A46" s="5">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="B46" s="7" t="s">
+      <c r="B46" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C46" s="7" t="s">
+      <c r="C46" s="5" t="s">
         <v>111</v>
       </c>
       <c r="H46" s="1" t="s">
@@ -2005,14 +2016,14 @@
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A47" s="7">
+      <c r="A47" s="5">
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-      <c r="B47" s="7" t="s">
+      <c r="B47" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C47" s="7" t="s">
+      <c r="C47" s="5" t="s">
         <v>24</v>
       </c>
       <c r="I47" s="1" t="s">
@@ -2020,14 +2031,14 @@
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A48" s="7">
+      <c r="A48" s="5">
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
-      <c r="B48" s="7" t="s">
+      <c r="B48" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C48" s="7" t="s">
+      <c r="C48" s="5" t="s">
         <v>84</v>
       </c>
       <c r="I48" s="1" t="s">
@@ -2035,14 +2046,14 @@
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A49" s="7">
+      <c r="A49" s="5">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="B49" s="7" t="s">
+      <c r="B49" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C49" s="7" t="s">
+      <c r="C49" s="5" t="s">
         <v>85</v>
       </c>
       <c r="I49" s="1" t="s">
@@ -2050,14 +2061,14 @@
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A50" s="7">
+      <c r="A50" s="5">
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
-      <c r="B50" s="7" t="s">
+      <c r="B50" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C50" s="7" t="s">
+      <c r="C50" s="5" t="s">
         <v>89</v>
       </c>
       <c r="I50" s="1" t="s">
@@ -2065,14 +2076,14 @@
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A51" s="7">
+      <c r="A51" s="5">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="B51" s="7" t="s">
+      <c r="B51" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C51" s="7" t="s">
+      <c r="C51" s="5" t="s">
         <v>91</v>
       </c>
       <c r="I51" s="1" t="s">
@@ -2080,14 +2091,14 @@
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A52" s="7">
+      <c r="A52" s="5">
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
-      <c r="B52" s="7" t="s">
+      <c r="B52" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C52" s="7" t="s">
+      <c r="C52" s="5" t="s">
         <v>92</v>
       </c>
       <c r="I52" s="1" t="s">
@@ -2095,14 +2106,14 @@
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A53" s="7">
+      <c r="A53" s="5">
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
-      <c r="B53" s="7" t="s">
+      <c r="B53" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C53" s="7" t="s">
+      <c r="C53" s="5" t="s">
         <v>93</v>
       </c>
       <c r="I53" s="1" t="s">
@@ -2110,14 +2121,14 @@
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A54" s="7">
+      <c r="A54" s="5">
         <f t="shared" si="0"/>
         <v>33</v>
       </c>
-      <c r="B54" s="7" t="s">
+      <c r="B54" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="C54" s="7" t="s">
+      <c r="C54" s="5" t="s">
         <v>94</v>
       </c>
       <c r="I54" s="1" t="s">
@@ -2125,14 +2136,14 @@
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A55" s="7">
+      <c r="A55" s="5">
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
-      <c r="B55" s="7" t="s">
+      <c r="B55" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="C55" s="7" t="s">
+      <c r="C55" s="5" t="s">
         <v>41</v>
       </c>
       <c r="I55" s="1" t="s">
@@ -2140,14 +2151,14 @@
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A56" s="7">
+      <c r="A56" s="5">
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
-      <c r="B56" s="7" t="s">
+      <c r="B56" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="C56" s="7" t="s">
+      <c r="C56" s="5" t="s">
         <v>43</v>
       </c>
       <c r="I56" s="1" t="s">
@@ -2155,14 +2166,14 @@
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A57" s="7">
+      <c r="A57" s="5">
         <f t="shared" si="0"/>
         <v>36</v>
       </c>
-      <c r="B57" s="7" t="s">
+      <c r="B57" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C57" s="7" t="s">
+      <c r="C57" s="5" t="s">
         <v>96</v>
       </c>
       <c r="I57" s="1" t="s">
@@ -2170,14 +2181,14 @@
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A58" s="7">
+      <c r="A58" s="5">
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="B58" s="7" t="s">
+      <c r="B58" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="C58" s="7" t="s">
+      <c r="C58" s="5" t="s">
         <v>97</v>
       </c>
       <c r="I58" s="1" t="s">
@@ -2185,14 +2196,14 @@
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A59" s="7">
+      <c r="A59" s="5">
         <f t="shared" si="0"/>
         <v>38</v>
       </c>
-      <c r="B59" s="7" t="s">
+      <c r="B59" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="C59" s="7" t="s">
+      <c r="C59" s="5" t="s">
         <v>99</v>
       </c>
       <c r="I59" s="1" t="s">
@@ -2200,14 +2211,14 @@
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A60" s="7">
+      <c r="A60" s="5">
         <f t="shared" si="0"/>
         <v>39</v>
       </c>
-      <c r="B60" s="7" t="s">
+      <c r="B60" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C60" s="7" t="s">
+      <c r="C60" s="5" t="s">
         <v>98</v>
       </c>
       <c r="I60" s="1" t="s">
@@ -2215,29 +2226,27 @@
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A61" s="7">
+      <c r="A61" s="5">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-      <c r="B61" s="7" t="s">
+      <c r="B61" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C61" s="7" t="s">
+      <c r="C61" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="I61" s="1" t="s">
-        <v>78</v>
-      </c>
+      <c r="I61" s="10"/>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A62" s="7">
+      <c r="A62" s="5">
         <f t="shared" si="0"/>
         <v>41</v>
       </c>
-      <c r="B62" s="7" t="s">
+      <c r="B62" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C62" s="7" t="s">
+      <c r="C62" s="5" t="s">
         <v>82</v>
       </c>
     </row>

</xml_diff>

<commit_message>
excel atualizado e formulas das calorias implementadas em excel. TODO: implementar funcao em activies
</commit_message>
<xml_diff>
--- a/others/activitiesClassification.xlsx
+++ b/others/activitiesClassification.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="124">
   <si>
     <t>Cycling, sport</t>
   </si>
@@ -385,12 +385,18 @@
   <si>
     <t>to 
 supress?</t>
+  </si>
+  <si>
+    <t>METS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -886,7 +892,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -906,6 +912,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -915,7 +924,7 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1260,63 +1269,68 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I62"/>
+  <dimension ref="A1:J62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="I61" sqref="I61"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="20.7109375" customWidth="1"/>
     <col min="3" max="3" width="29.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="9" width="10.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="10" width="10.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="E1" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="F1" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-    </row>
-    <row r="2" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="3" t="s">
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+    </row>
+    <row r="2" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="8"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="G2" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="I2" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="J2" s="3" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>-1</v>
       </c>
@@ -1326,14 +1340,15 @@
       <c r="C3" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D3" s="5"/>
+      <c r="E3" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>-1</v>
       </c>
@@ -1343,14 +1358,15 @@
       <c r="C4" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D4" s="5"/>
+      <c r="E4" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>-1</v>
       </c>
@@ -1360,14 +1376,15 @@
       <c r="C5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D5" s="5"/>
+      <c r="E5" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>-1</v>
       </c>
@@ -1377,14 +1394,15 @@
       <c r="C6" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>78</v>
-      </c>
+      <c r="D6" s="5"/>
       <c r="E6" s="1" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F6" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>-1</v>
       </c>
@@ -1394,14 +1412,15 @@
       <c r="C7" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>78</v>
-      </c>
+      <c r="D7" s="5"/>
       <c r="E7" s="1" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F7" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>-1</v>
       </c>
@@ -1411,14 +1430,15 @@
       <c r="C8" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D8" s="5"/>
+      <c r="E8" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>-1</v>
       </c>
@@ -1428,14 +1448,15 @@
       <c r="C9" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D9" s="5"/>
+      <c r="E9" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>-1</v>
       </c>
@@ -1445,14 +1466,15 @@
       <c r="C10" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D10" s="5"/>
+      <c r="E10" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>-1</v>
       </c>
@@ -1462,14 +1484,15 @@
       <c r="C11" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>78</v>
-      </c>
+      <c r="D11" s="5"/>
       <c r="E11" s="1" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F11" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>-1</v>
       </c>
@@ -1479,14 +1502,15 @@
       <c r="C12" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D12" s="5"/>
+      <c r="E12" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>-1</v>
       </c>
@@ -1496,14 +1520,15 @@
       <c r="C13" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="D13" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D13" s="5"/>
+      <c r="E13" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>-1</v>
       </c>
@@ -1513,14 +1538,15 @@
       <c r="C14" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>78</v>
-      </c>
+      <c r="D14" s="5"/>
       <c r="E14" s="1" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F14" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>-1</v>
       </c>
@@ -1530,14 +1556,15 @@
       <c r="C15" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="D15" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D15" s="5"/>
+      <c r="E15" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>-1</v>
       </c>
@@ -1547,14 +1574,15 @@
       <c r="C16" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="D16" s="1" t="s">
-        <v>78</v>
-      </c>
+      <c r="D16" s="5"/>
       <c r="E16" s="1" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F16" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>-1</v>
       </c>
@@ -1564,14 +1592,15 @@
       <c r="C17" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="D17" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D17" s="5"/>
+      <c r="E17" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>-1</v>
       </c>
@@ -1581,14 +1610,15 @@
       <c r="C18" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="D18" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D18" s="5"/>
+      <c r="E18" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>-1</v>
       </c>
@@ -1598,14 +1628,15 @@
       <c r="C19" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="D19" s="1" t="s">
-        <v>78</v>
-      </c>
+      <c r="D19" s="5"/>
       <c r="E19" s="1" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F19" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="6">
         <v>-1</v>
       </c>
@@ -1615,18 +1646,19 @@
       <c r="C20" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="D20" s="2" t="s">
-        <v>78</v>
-      </c>
+      <c r="D20" s="6"/>
       <c r="E20" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="F20" s="2"/>
+      <c r="F20" s="2" t="s">
+        <v>78</v>
+      </c>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J20" s="2"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
         <v>0</v>
       </c>
@@ -1636,11 +1668,14 @@
       <c r="C21" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="E21" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D21" s="11">
+        <v>5.3</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
         <f>A21+1</f>
         <v>1</v>
@@ -1651,11 +1686,14 @@
       <c r="C22" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="E22" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D22" s="11">
+        <v>5.8</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
         <f t="shared" ref="A23:A62" si="0">A22+1</f>
         <v>2</v>
@@ -1666,11 +1704,14 @@
       <c r="C23" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="E23" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D23" s="11">
+        <v>3</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -1681,11 +1722,14 @@
       <c r="C24" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E24" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D24" s="11">
+        <v>3</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1696,11 +1740,14 @@
       <c r="C25" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="E25" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D25" s="11">
+        <v>3.5</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1711,11 +1758,14 @@
       <c r="C26" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="E26" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D26" s="11">
+        <v>9</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1726,11 +1776,14 @@
       <c r="C27" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="E27" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D27" s="11">
+        <v>5.8</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1741,11 +1794,14 @@
       <c r="C28" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="E28" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D28" s="11">
+        <v>5</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1756,11 +1812,14 @@
       <c r="C29" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="F29" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D29" s="11">
+        <v>7</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1771,11 +1830,14 @@
       <c r="C30" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="F30" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D30" s="11">
+        <v>7.5</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="5">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1786,11 +1848,14 @@
       <c r="C31" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="F31" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D31" s="11">
+        <v>8.5</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="5">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1801,11 +1866,14 @@
       <c r="C32" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="F32" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D32" s="11">
+        <v>7</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="5">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1816,11 +1884,14 @@
       <c r="C33" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="F33" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D33" s="11">
+        <v>6</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="5">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1831,11 +1902,14 @@
       <c r="C34" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="G34" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D34" s="11">
+        <v>7</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="5">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1846,11 +1920,14 @@
       <c r="C35" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="G35" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D35" s="11">
+        <v>5.3</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="5">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1861,11 +1938,14 @@
       <c r="C36" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="G36" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D36" s="11">
+        <v>4.8</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="5">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1876,11 +1956,14 @@
       <c r="C37" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="G37" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D37" s="11">
+        <v>5.5</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="5">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1891,11 +1974,14 @@
       <c r="C38" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="G38" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D38" s="11">
+        <v>3.8</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="5">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -1906,11 +1992,14 @@
       <c r="C39" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="G39" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D39" s="11">
+        <v>3</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="5">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -1921,11 +2010,14 @@
       <c r="C40" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="H40" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D40" s="11">
+        <v>7.3</v>
+      </c>
+      <c r="I40" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="5">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -1936,11 +2028,14 @@
       <c r="C41" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="H41" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D41" s="11">
+        <v>7.8</v>
+      </c>
+      <c r="I41" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="5">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -1951,11 +2046,14 @@
       <c r="C42" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="H42" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D42" s="11">
+        <v>3</v>
+      </c>
+      <c r="I42" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="5">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -1966,11 +2064,14 @@
       <c r="C43" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="H43" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D43" s="11">
+        <v>7</v>
+      </c>
+      <c r="I43" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="5">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -1981,11 +2082,14 @@
       <c r="C44" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="H44" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D44" s="11">
+        <v>4</v>
+      </c>
+      <c r="I44" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="5">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -1996,11 +2100,14 @@
       <c r="C45" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="H45" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D45" s="11">
+        <v>5</v>
+      </c>
+      <c r="I45" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="5">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -2011,11 +2118,14 @@
       <c r="C46" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="H46" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D46" s="11">
+        <v>8</v>
+      </c>
+      <c r="I46" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="5">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -2026,11 +2136,14 @@
       <c r="C47" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="I47" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D47" s="11">
+        <v>5.5</v>
+      </c>
+      <c r="J47" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="5">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -2041,11 +2154,14 @@
       <c r="C48" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="I48" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D48" s="11">
+        <v>6.5</v>
+      </c>
+      <c r="J48" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="5">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -2056,11 +2172,14 @@
       <c r="C49" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="I49" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D49" s="11">
+        <v>12.8</v>
+      </c>
+      <c r="J49" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="5">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -2071,11 +2190,14 @@
       <c r="C50" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="I50" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D50" s="11">
+        <v>6</v>
+      </c>
+      <c r="J50" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="5">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -2086,11 +2208,14 @@
       <c r="C51" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="I51" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D51" s="11">
+        <v>6.3</v>
+      </c>
+      <c r="J51" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="5">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -2101,11 +2226,14 @@
       <c r="C52" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="I52" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D52" s="11">
+        <v>7</v>
+      </c>
+      <c r="J52" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="5">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -2116,11 +2244,14 @@
       <c r="C53" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="I53" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D53" s="11">
+        <v>8</v>
+      </c>
+      <c r="J53" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="5">
         <f t="shared" si="0"/>
         <v>33</v>
@@ -2131,11 +2262,14 @@
       <c r="C54" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="I54" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D54" s="11">
+        <v>7.8</v>
+      </c>
+      <c r="J54" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="5">
         <f t="shared" si="0"/>
         <v>34</v>
@@ -2146,11 +2280,14 @@
       <c r="C55" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="I55" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D55" s="11">
+        <v>8</v>
+      </c>
+      <c r="J55" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="5">
         <f t="shared" si="0"/>
         <v>35</v>
@@ -2161,11 +2298,14 @@
       <c r="C56" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="I56" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D56" s="11">
+        <v>7.3</v>
+      </c>
+      <c r="J56" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="5">
         <f t="shared" si="0"/>
         <v>36</v>
@@ -2176,11 +2316,14 @@
       <c r="C57" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="I57" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D57" s="11">
+        <v>4</v>
+      </c>
+      <c r="J57" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="5">
         <f t="shared" si="0"/>
         <v>37</v>
@@ -2191,11 +2334,14 @@
       <c r="C58" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="I58" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D58" s="11">
+        <v>7.3</v>
+      </c>
+      <c r="J58" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="5">
         <f t="shared" si="0"/>
         <v>38</v>
@@ -2206,11 +2352,14 @@
       <c r="C59" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="I59" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D59" s="11">
+        <v>8</v>
+      </c>
+      <c r="J59" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="5">
         <f t="shared" si="0"/>
         <v>39</v>
@@ -2221,11 +2370,14 @@
       <c r="C60" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="I60" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D60" s="11">
+        <v>4</v>
+      </c>
+      <c r="J60" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="5">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -2236,9 +2388,12 @@
       <c r="C61" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="I61" s="10"/>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D61" s="11">
+        <v>10.3</v>
+      </c>
+      <c r="J61" s="7"/>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="5">
         <f t="shared" si="0"/>
         <v>41</v>
@@ -2249,17 +2404,19 @@
       <c r="C62" s="5" t="s">
         <v>82</v>
       </c>
+      <c r="D62" s="11"/>
     </row>
   </sheetData>
-  <sortState ref="A21:F33">
-    <sortCondition ref="E21:E33"/>
+  <sortState ref="A21:G33">
+    <sortCondition ref="F21:F33"/>
   </sortState>
-  <mergeCells count="5">
+  <mergeCells count="6">
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:J1"/>
     <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:I1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
divisao de tarefas + **definicao de recordes**
</commit_message>
<xml_diff>
--- a/others/activitiesClassification.xlsx
+++ b/others/activitiesClassification.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="127">
   <si>
     <t>Cycling, sport</t>
   </si>
@@ -388,6 +388,15 @@
   </si>
   <si>
     <t>METS</t>
+  </si>
+  <si>
+    <t>Oliveira</t>
+  </si>
+  <si>
+    <t>Santos</t>
+  </si>
+  <si>
+    <t>Camposinhos</t>
   </si>
 </sst>
 </file>
@@ -397,7 +406,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -529,14 +538,6 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -912,7 +913,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -924,7 +925,7 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1269,10 +1270,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J62"/>
+  <dimension ref="A1:K62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" topLeftCell="B34" workbookViewId="0">
+      <selection activeCell="I55" sqref="I55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1582,7 +1583,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>-1</v>
       </c>
@@ -1600,7 +1601,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>-1</v>
       </c>
@@ -1618,7 +1619,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>-1</v>
       </c>
@@ -1636,7 +1637,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="6">
         <v>-1</v>
       </c>
@@ -1658,7 +1659,7 @@
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
         <v>0</v>
       </c>
@@ -1668,14 +1669,17 @@
       <c r="C21" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="D21" s="11">
+      <c r="D21" s="7">
         <v>5.3</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K21" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
         <f>A21+1</f>
         <v>1</v>
@@ -1686,14 +1690,17 @@
       <c r="C22" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="D22" s="11">
+      <c r="D22" s="7">
         <v>5.8</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K22" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
         <f t="shared" ref="A23:A62" si="0">A22+1</f>
         <v>2</v>
@@ -1704,14 +1711,17 @@
       <c r="C23" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="D23" s="11">
+      <c r="D23" s="7">
         <v>3</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K23" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -1722,14 +1732,17 @@
       <c r="C24" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D24" s="11">
+      <c r="D24" s="7">
         <v>3</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K24" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1740,14 +1753,17 @@
       <c r="C25" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="D25" s="11">
+      <c r="D25" s="7">
         <v>3.5</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K25" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1758,14 +1774,17 @@
       <c r="C26" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="D26" s="11">
+      <c r="D26" s="7">
         <v>9</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K26" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1776,14 +1795,17 @@
       <c r="C27" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="D27" s="11">
+      <c r="D27" s="7">
         <v>5.8</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K27" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1794,14 +1816,17 @@
       <c r="C28" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="D28" s="11">
+      <c r="D28" s="7">
         <v>5</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K28" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1812,14 +1837,17 @@
       <c r="C29" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="D29" s="11">
+      <c r="D29" s="7">
         <v>7</v>
       </c>
       <c r="G29" s="1" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K29" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1830,14 +1858,17 @@
       <c r="C30" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="D30" s="11">
+      <c r="D30" s="7">
         <v>7.5</v>
       </c>
       <c r="G30" s="1" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K30" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="5">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1848,14 +1879,17 @@
       <c r="C31" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="D31" s="11">
+      <c r="D31" s="7">
         <v>8.5</v>
       </c>
       <c r="G31" s="1" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K31" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="5">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1866,14 +1900,17 @@
       <c r="C32" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="D32" s="11">
+      <c r="D32" s="7">
         <v>7</v>
       </c>
       <c r="G32" s="1" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K32" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="5">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1884,14 +1921,17 @@
       <c r="C33" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="D33" s="11">
+      <c r="D33" s="7">
         <v>6</v>
       </c>
       <c r="G33" s="1" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K33" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="5">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1902,14 +1942,17 @@
       <c r="C34" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="D34" s="11">
+      <c r="D34" s="7">
         <v>7</v>
       </c>
       <c r="H34" s="1" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K34" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="5">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1920,14 +1963,17 @@
       <c r="C35" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="D35" s="11">
+      <c r="D35" s="7">
         <v>5.3</v>
       </c>
       <c r="H35" s="1" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K35" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="5">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1938,14 +1984,17 @@
       <c r="C36" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="D36" s="11">
+      <c r="D36" s="7">
         <v>4.8</v>
       </c>
       <c r="H36" s="1" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K36" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="5">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1956,14 +2005,17 @@
       <c r="C37" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="D37" s="11">
+      <c r="D37" s="7">
         <v>5.5</v>
       </c>
       <c r="H37" s="1" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K37" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="5">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1974,14 +2026,17 @@
       <c r="C38" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="D38" s="11">
+      <c r="D38" s="7">
         <v>3.8</v>
       </c>
       <c r="H38" s="1" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K38" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="5">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -1992,14 +2047,17 @@
       <c r="C39" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="D39" s="11">
+      <c r="D39" s="7">
         <v>3</v>
       </c>
       <c r="H39" s="1" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K39" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="5">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -2010,14 +2068,17 @@
       <c r="C40" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="D40" s="11">
+      <c r="D40" s="7">
         <v>7.3</v>
       </c>
       <c r="I40" s="1" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K40" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="5">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -2028,14 +2089,17 @@
       <c r="C41" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="D41" s="11">
+      <c r="D41" s="7">
         <v>7.8</v>
       </c>
       <c r="I41" s="1" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K41" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="5">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -2046,14 +2110,17 @@
       <c r="C42" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="D42" s="11">
+      <c r="D42" s="7">
         <v>3</v>
       </c>
       <c r="I42" s="1" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K42" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="5">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -2064,14 +2131,17 @@
       <c r="C43" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="D43" s="11">
+      <c r="D43" s="7">
         <v>7</v>
       </c>
       <c r="I43" s="1" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K43" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="5">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -2082,14 +2152,17 @@
       <c r="C44" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="D44" s="11">
+      <c r="D44" s="7">
         <v>4</v>
       </c>
       <c r="I44" s="1" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K44" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="5">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -2100,14 +2173,17 @@
       <c r="C45" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="D45" s="11">
+      <c r="D45" s="7">
         <v>5</v>
       </c>
       <c r="I45" s="1" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K45" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="5">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -2118,14 +2194,17 @@
       <c r="C46" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="D46" s="11">
+      <c r="D46" s="7">
         <v>8</v>
       </c>
       <c r="I46" s="1" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K46" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="5">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -2136,14 +2215,17 @@
       <c r="C47" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D47" s="11">
+      <c r="D47" s="7">
         <v>5.5</v>
       </c>
       <c r="J47" s="1" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K47" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="5">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -2154,14 +2236,17 @@
       <c r="C48" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="D48" s="11">
+      <c r="D48" s="7">
         <v>6.5</v>
       </c>
       <c r="J48" s="1" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K48" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="5">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -2172,14 +2257,17 @@
       <c r="C49" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="D49" s="11">
+      <c r="D49" s="7">
         <v>12.8</v>
       </c>
       <c r="J49" s="1" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K49" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="5">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -2190,14 +2278,17 @@
       <c r="C50" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="D50" s="11">
+      <c r="D50" s="7">
         <v>6</v>
       </c>
       <c r="J50" s="1" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K50" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="5">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -2208,14 +2299,17 @@
       <c r="C51" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="D51" s="11">
+      <c r="D51" s="7">
         <v>6.3</v>
       </c>
       <c r="J51" s="1" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K51" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="5">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -2226,14 +2320,17 @@
       <c r="C52" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="D52" s="11">
+      <c r="D52" s="7">
         <v>7</v>
       </c>
       <c r="J52" s="1" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K52" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="5">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -2244,14 +2341,17 @@
       <c r="C53" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="D53" s="11">
+      <c r="D53" s="7">
         <v>8</v>
       </c>
       <c r="J53" s="1" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K53" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="5">
         <f t="shared" si="0"/>
         <v>33</v>
@@ -2262,14 +2362,17 @@
       <c r="C54" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="D54" s="11">
+      <c r="D54" s="7">
         <v>7.8</v>
       </c>
       <c r="J54" s="1" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K54" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="5">
         <f t="shared" si="0"/>
         <v>34</v>
@@ -2280,14 +2383,17 @@
       <c r="C55" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="D55" s="11">
+      <c r="D55" s="7">
         <v>8</v>
       </c>
       <c r="J55" s="1" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K55" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="5">
         <f t="shared" si="0"/>
         <v>35</v>
@@ -2298,14 +2404,17 @@
       <c r="C56" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="D56" s="11">
+      <c r="D56" s="7">
         <v>7.3</v>
       </c>
       <c r="J56" s="1" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K56" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="5">
         <f t="shared" si="0"/>
         <v>36</v>
@@ -2316,14 +2425,17 @@
       <c r="C57" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="D57" s="11">
+      <c r="D57" s="7">
         <v>4</v>
       </c>
       <c r="J57" s="1" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K57" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="5">
         <f t="shared" si="0"/>
         <v>37</v>
@@ -2334,14 +2446,17 @@
       <c r="C58" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="D58" s="11">
+      <c r="D58" s="7">
         <v>7.3</v>
       </c>
       <c r="J58" s="1" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K58" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" s="5">
         <f t="shared" si="0"/>
         <v>38</v>
@@ -2352,14 +2467,17 @@
       <c r="C59" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="D59" s="11">
+      <c r="D59" s="7">
         <v>8</v>
       </c>
       <c r="J59" s="1" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K59" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" s="5">
         <f t="shared" si="0"/>
         <v>39</v>
@@ -2370,14 +2488,17 @@
       <c r="C60" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="D60" s="11">
+      <c r="D60" s="7">
         <v>4</v>
       </c>
       <c r="J60" s="1" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K60" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" s="5">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -2388,12 +2509,17 @@
       <c r="C61" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="D61" s="11">
+      <c r="D61" s="7">
         <v>10.3</v>
       </c>
-      <c r="J61" s="7"/>
-    </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J61" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="K61" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" s="5">
         <f t="shared" si="0"/>
         <v>41</v>
@@ -2404,7 +2530,7 @@
       <c r="C62" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="D62" s="11"/>
+      <c r="D62" s="7"/>
     </row>
   </sheetData>
   <sortState ref="A21:G33">

</xml_diff>

<commit_message>
done nas tarefas do excel
</commit_message>
<xml_diff>
--- a/others/activitiesClassification.xlsx
+++ b/others/activitiesClassification.xlsx
@@ -9,6 +9,9 @@
   <sheets>
     <sheet name="car" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">car!$B$21:$K$62</definedName>
+  </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
@@ -396,7 +399,7 @@
     <t>Santos</t>
   </si>
   <si>
-    <t>Camposinhos</t>
+    <t>Camposinhos --- DONE</t>
   </si>
 </sst>
 </file>
@@ -916,6 +919,9 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -923,9 +929,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1272,8 +1275,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B34" workbookViewId="0">
-      <selection activeCell="I55" sqref="I55"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1286,35 +1289,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="11" t="s">
         <v>123</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
     </row>
     <row r="2" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="8"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
+      <c r="A2" s="9"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
       <c r="F2" s="3" t="s">
         <v>114</v>
       </c>
@@ -2512,7 +2515,7 @@
       <c r="D61" s="7">
         <v>10.3</v>
       </c>
-      <c r="J61" s="11" t="s">
+      <c r="J61" s="8" t="s">
         <v>78</v>
       </c>
       <c r="K61" t="s">

</xml_diff>

<commit_message>
Actualizaçao excel com valores das intensidades.
</commit_message>
<xml_diff>
--- a/others/activitiesClassification.xlsx
+++ b/others/activitiesClassification.xlsx
@@ -10,14 +10,14 @@
     <sheet name="car" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">car!$B$21:$K$62</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">car!$B$21:$L$62</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="128">
   <si>
     <t>Cycling, sport</t>
   </si>
@@ -400,6 +400,9 @@
   </si>
   <si>
     <t>Camposinhos --- DONE</t>
+  </si>
+  <si>
+    <t>Intens. (mins)</t>
   </si>
 </sst>
 </file>
@@ -896,7 +899,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -929,6 +932,10 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1273,10 +1280,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K62"/>
+  <dimension ref="A1:O62"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1284,11 +1291,12 @@
     <col min="2" max="2" width="20.7109375" customWidth="1"/>
     <col min="3" max="3" width="29.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="10" width="10.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="7.85546875" customWidth="1"/>
+    <col min="6" max="6" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="11" width="10.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>59</v>
       </c>
@@ -1302,39 +1310,43 @@
         <v>123</v>
       </c>
       <c r="E1" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="G1" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="G1" s="11"/>
       <c r="H1" s="11"/>
       <c r="I1" s="11"/>
       <c r="J1" s="11"/>
-    </row>
-    <row r="2" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K1" s="11"/>
+    </row>
+    <row r="2" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="9"/>
       <c r="B2" s="9"/>
       <c r="C2" s="9"/>
       <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="3" t="s">
+      <c r="E2" s="10"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="H2" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="I2" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="J2" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="K2" s="3" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>-1</v>
       </c>
@@ -1345,14 +1357,15 @@
         <v>64</v>
       </c>
       <c r="D3" s="5"/>
-      <c r="E3" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E3" s="5"/>
+      <c r="F3" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>-1</v>
       </c>
@@ -1363,14 +1376,15 @@
         <v>68</v>
       </c>
       <c r="D4" s="5"/>
-      <c r="E4" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E4" s="5"/>
+      <c r="F4" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>-1</v>
       </c>
@@ -1381,14 +1395,15 @@
         <v>7</v>
       </c>
       <c r="D5" s="5"/>
-      <c r="E5" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E5" s="5"/>
+      <c r="F5" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>-1</v>
       </c>
@@ -1399,14 +1414,15 @@
         <v>119</v>
       </c>
       <c r="D6" s="5"/>
-      <c r="E6" s="1" t="s">
-        <v>78</v>
-      </c>
+      <c r="E6" s="5"/>
       <c r="F6" s="1" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G6" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>-1</v>
       </c>
@@ -1417,14 +1433,15 @@
         <v>81</v>
       </c>
       <c r="D7" s="5"/>
-      <c r="E7" s="1" t="s">
-        <v>78</v>
-      </c>
+      <c r="E7" s="5"/>
       <c r="F7" s="1" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G7" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>-1</v>
       </c>
@@ -1435,14 +1452,15 @@
         <v>25</v>
       </c>
       <c r="D8" s="5"/>
-      <c r="E8" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E8" s="5"/>
+      <c r="F8" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>-1</v>
       </c>
@@ -1453,14 +1471,15 @@
         <v>86</v>
       </c>
       <c r="D9" s="5"/>
-      <c r="E9" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E9" s="5"/>
+      <c r="F9" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>-1</v>
       </c>
@@ -1471,14 +1490,15 @@
         <v>29</v>
       </c>
       <c r="D10" s="5"/>
-      <c r="E10" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E10" s="5"/>
+      <c r="F10" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>-1</v>
       </c>
@@ -1489,14 +1509,15 @@
         <v>87</v>
       </c>
       <c r="D11" s="5"/>
-      <c r="E11" s="1" t="s">
-        <v>78</v>
-      </c>
+      <c r="E11" s="5"/>
       <c r="F11" s="1" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G11" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>-1</v>
       </c>
@@ -1507,14 +1528,15 @@
         <v>90</v>
       </c>
       <c r="D12" s="5"/>
-      <c r="E12" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="J12" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E12" s="5"/>
+      <c r="F12" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>-1</v>
       </c>
@@ -1525,14 +1547,15 @@
         <v>100</v>
       </c>
       <c r="D13" s="5"/>
-      <c r="E13" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="J13" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E13" s="5"/>
+      <c r="F13" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>-1</v>
       </c>
@@ -1543,14 +1566,15 @@
         <v>104</v>
       </c>
       <c r="D14" s="5"/>
-      <c r="E14" s="1" t="s">
-        <v>78</v>
-      </c>
+      <c r="E14" s="5"/>
       <c r="F14" s="1" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G14" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>-1</v>
       </c>
@@ -1561,14 +1585,15 @@
         <v>105</v>
       </c>
       <c r="D15" s="5"/>
-      <c r="E15" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="J15" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E15" s="5"/>
+      <c r="F15" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>-1</v>
       </c>
@@ -1579,14 +1604,15 @@
         <v>106</v>
       </c>
       <c r="D16" s="5"/>
-      <c r="E16" s="1" t="s">
-        <v>78</v>
-      </c>
+      <c r="E16" s="5"/>
       <c r="F16" s="1" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G16" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>-1</v>
       </c>
@@ -1597,14 +1623,15 @@
         <v>107</v>
       </c>
       <c r="D17" s="5"/>
-      <c r="E17" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E17" s="5"/>
+      <c r="F17" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>-1</v>
       </c>
@@ -1615,14 +1642,15 @@
         <v>109</v>
       </c>
       <c r="D18" s="5"/>
-      <c r="E18" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E18" s="5"/>
+      <c r="F18" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>-1</v>
       </c>
@@ -1633,14 +1661,15 @@
         <v>110</v>
       </c>
       <c r="D19" s="5"/>
-      <c r="E19" s="1" t="s">
-        <v>78</v>
-      </c>
+      <c r="E19" s="5"/>
       <c r="F19" s="1" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G19" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="6">
         <v>-1</v>
       </c>
@@ -1651,18 +1680,19 @@
         <v>112</v>
       </c>
       <c r="D20" s="6"/>
-      <c r="E20" s="2" t="s">
-        <v>78</v>
-      </c>
+      <c r="E20" s="6"/>
       <c r="F20" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="G20" s="2"/>
+      <c r="G20" s="2" t="s">
+        <v>78</v>
+      </c>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K20" s="2"/>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
         <v>0</v>
       </c>
@@ -1675,14 +1705,19 @@
       <c r="D21" s="7">
         <v>5.3</v>
       </c>
-      <c r="F21" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="K21" t="s">
+      <c r="E21" s="13">
+        <v>119</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="L21" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="N21" s="12"/>
+      <c r="O21" s="12"/>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
         <f>A21+1</f>
         <v>1</v>
@@ -1696,14 +1731,19 @@
       <c r="D22" s="7">
         <v>5.8</v>
       </c>
-      <c r="F22" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="K22" t="s">
+      <c r="E22" s="13">
+        <v>109</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="L22" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="N22" s="12"/>
+      <c r="O22" s="12"/>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
         <f t="shared" ref="A23:A62" si="0">A22+1</f>
         <v>2</v>
@@ -1717,14 +1757,19 @@
       <c r="D23" s="7">
         <v>3</v>
       </c>
-      <c r="F23" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="K23" t="s">
+      <c r="E23" s="13">
+        <v>210</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="L23" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="N23" s="12"/>
+      <c r="O23" s="12"/>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -1738,14 +1783,19 @@
       <c r="D24" s="7">
         <v>3</v>
       </c>
-      <c r="F24" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="K24" t="s">
+      <c r="E24" s="13">
+        <v>210</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="L24" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="N24" s="12"/>
+      <c r="O24" s="12"/>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1759,14 +1809,19 @@
       <c r="D25" s="7">
         <v>3.5</v>
       </c>
-      <c r="F25" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="K25" t="s">
+      <c r="E25" s="13">
+        <v>180</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="L25" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="N25" s="12"/>
+      <c r="O25" s="12"/>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1780,14 +1835,19 @@
       <c r="D26" s="7">
         <v>9</v>
       </c>
-      <c r="F26" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="K26" t="s">
+      <c r="E26" s="13">
+        <v>70</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="L26" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="N26" s="12"/>
+      <c r="O26" s="12"/>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1801,14 +1861,19 @@
       <c r="D27" s="7">
         <v>5.8</v>
       </c>
-      <c r="F27" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="K27" t="s">
+      <c r="E27" s="13">
+        <v>109</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="L27" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="N27" s="12"/>
+      <c r="O27" s="12"/>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1822,14 +1887,19 @@
       <c r="D28" s="7">
         <v>5</v>
       </c>
-      <c r="F28" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="K28" t="s">
+      <c r="E28" s="13">
+        <v>126</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="L28" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="N28" s="12"/>
+      <c r="O28" s="12"/>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1843,14 +1913,19 @@
       <c r="D29" s="7">
         <v>7</v>
       </c>
-      <c r="G29" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="K29" t="s">
+      <c r="E29" s="13">
+        <v>90</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="L29" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="N29" s="12"/>
+      <c r="O29" s="12"/>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1864,14 +1939,19 @@
       <c r="D30" s="7">
         <v>7.5</v>
       </c>
-      <c r="G30" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="K30" t="s">
+      <c r="E30" s="13">
+        <v>84</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="L30" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="N30" s="12"/>
+      <c r="O30" s="12"/>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="5">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1885,14 +1965,19 @@
       <c r="D31" s="7">
         <v>8.5</v>
       </c>
-      <c r="G31" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="K31" t="s">
+      <c r="E31" s="13">
+        <v>74</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="L31" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="N31" s="12"/>
+      <c r="O31" s="12"/>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="5">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1906,14 +1991,19 @@
       <c r="D32" s="7">
         <v>7</v>
       </c>
-      <c r="G32" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="K32" t="s">
+      <c r="E32" s="13">
+        <v>90</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="L32" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="N32" s="12"/>
+      <c r="O32" s="12"/>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" s="5">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1927,14 +2017,19 @@
       <c r="D33" s="7">
         <v>6</v>
       </c>
-      <c r="G33" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="K33" t="s">
+      <c r="E33" s="13">
+        <v>105</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="L33" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="N33" s="12"/>
+      <c r="O33" s="12"/>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" s="5">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1948,14 +2043,19 @@
       <c r="D34" s="7">
         <v>7</v>
       </c>
-      <c r="H34" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="K34" t="s">
+      <c r="E34" s="13">
+        <v>90</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="L34" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="N34" s="12"/>
+      <c r="O34" s="12"/>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" s="5">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1969,14 +2069,19 @@
       <c r="D35" s="7">
         <v>5.3</v>
       </c>
-      <c r="H35" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="K35" t="s">
+      <c r="E35" s="13">
+        <v>119</v>
+      </c>
+      <c r="I35" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="L35" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="N35" s="12"/>
+      <c r="O35" s="12"/>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" s="5">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1990,14 +2095,19 @@
       <c r="D36" s="7">
         <v>4.8</v>
       </c>
-      <c r="H36" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="K36" t="s">
+      <c r="E36" s="13">
+        <v>131</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="L36" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="N36" s="12"/>
+      <c r="O36" s="12"/>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" s="5">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -2011,14 +2121,19 @@
       <c r="D37" s="7">
         <v>5.5</v>
       </c>
-      <c r="H37" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="K37" t="s">
+      <c r="E37" s="13">
+        <v>115</v>
+      </c>
+      <c r="I37" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="L37" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="N37" s="12"/>
+      <c r="O37" s="12"/>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38" s="5">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -2032,14 +2147,19 @@
       <c r="D38" s="7">
         <v>3.8</v>
       </c>
-      <c r="H38" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="K38" t="s">
+      <c r="E38" s="13">
+        <v>166</v>
+      </c>
+      <c r="I38" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="L38" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="N38" s="12"/>
+      <c r="O38" s="12"/>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39" s="5">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -2053,14 +2173,19 @@
       <c r="D39" s="7">
         <v>3</v>
       </c>
-      <c r="H39" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="K39" t="s">
+      <c r="E39" s="13">
+        <v>210</v>
+      </c>
+      <c r="I39" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="L39" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="N39" s="12"/>
+      <c r="O39" s="12"/>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40" s="5">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -2074,14 +2199,19 @@
       <c r="D40" s="7">
         <v>7.3</v>
       </c>
-      <c r="I40" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="K40" t="s">
+      <c r="E40" s="13">
+        <v>86</v>
+      </c>
+      <c r="J40" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="L40" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="N40" s="12"/>
+      <c r="O40" s="12"/>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41" s="5">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -2095,14 +2225,19 @@
       <c r="D41" s="7">
         <v>7.8</v>
       </c>
-      <c r="I41" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="K41" t="s">
+      <c r="E41" s="13">
+        <v>81</v>
+      </c>
+      <c r="J41" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="L41" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="N41" s="12"/>
+      <c r="O41" s="12"/>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A42" s="5">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -2116,14 +2251,19 @@
       <c r="D42" s="7">
         <v>3</v>
       </c>
-      <c r="I42" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="K42" t="s">
+      <c r="E42" s="13">
+        <v>210</v>
+      </c>
+      <c r="J42" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="L42" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="N42" s="12"/>
+      <c r="O42" s="12"/>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43" s="5">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -2137,14 +2277,19 @@
       <c r="D43" s="7">
         <v>7</v>
       </c>
-      <c r="I43" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="K43" t="s">
+      <c r="E43" s="13">
+        <v>90</v>
+      </c>
+      <c r="J43" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="L43" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="N43" s="12"/>
+      <c r="O43" s="12"/>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A44" s="5">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -2158,14 +2303,19 @@
       <c r="D44" s="7">
         <v>4</v>
       </c>
-      <c r="I44" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="K44" t="s">
+      <c r="E44" s="13">
+        <v>158</v>
+      </c>
+      <c r="J44" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="L44" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="N44" s="12"/>
+      <c r="O44" s="12"/>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A45" s="5">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -2179,14 +2329,19 @@
       <c r="D45" s="7">
         <v>5</v>
       </c>
-      <c r="I45" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="K45" t="s">
+      <c r="E45" s="13">
+        <v>126</v>
+      </c>
+      <c r="J45" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="L45" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="N45" s="12"/>
+      <c r="O45" s="12"/>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A46" s="5">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -2200,14 +2355,19 @@
       <c r="D46" s="7">
         <v>8</v>
       </c>
-      <c r="I46" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="K46" t="s">
+      <c r="E46" s="13">
+        <v>79</v>
+      </c>
+      <c r="J46" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="L46" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="N46" s="12"/>
+      <c r="O46" s="12"/>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47" s="5">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -2221,14 +2381,19 @@
       <c r="D47" s="7">
         <v>5.5</v>
       </c>
-      <c r="J47" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="K47" t="s">
+      <c r="E47" s="13">
+        <v>115</v>
+      </c>
+      <c r="K47" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="L47" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="N47" s="12"/>
+      <c r="O47" s="12"/>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A48" s="5">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -2242,14 +2407,19 @@
       <c r="D48" s="7">
         <v>6.5</v>
       </c>
-      <c r="J48" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="K48" t="s">
+      <c r="E48" s="13">
+        <v>97</v>
+      </c>
+      <c r="K48" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="L48" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="N48" s="12"/>
+      <c r="O48" s="12"/>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A49" s="5">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -2263,14 +2433,19 @@
       <c r="D49" s="7">
         <v>12.8</v>
       </c>
-      <c r="J49" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="K49" t="s">
+      <c r="E49" s="13">
+        <v>49</v>
+      </c>
+      <c r="K49" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="L49" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="N49" s="12"/>
+      <c r="O49" s="12"/>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A50" s="5">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -2284,14 +2459,19 @@
       <c r="D50" s="7">
         <v>6</v>
       </c>
-      <c r="J50" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="K50" t="s">
+      <c r="E50" s="13">
+        <v>105</v>
+      </c>
+      <c r="K50" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="L50" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="N50" s="12"/>
+      <c r="O50" s="12"/>
+    </row>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A51" s="5">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -2305,14 +2485,19 @@
       <c r="D51" s="7">
         <v>6.3</v>
       </c>
-      <c r="J51" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="K51" t="s">
+      <c r="E51" s="13">
+        <v>100</v>
+      </c>
+      <c r="K51" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="L51" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="N51" s="12"/>
+      <c r="O51" s="12"/>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A52" s="5">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -2326,14 +2511,19 @@
       <c r="D52" s="7">
         <v>7</v>
       </c>
-      <c r="J52" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="K52" t="s">
+      <c r="E52" s="13">
+        <v>90</v>
+      </c>
+      <c r="K52" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="L52" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="N52" s="12"/>
+      <c r="O52" s="12"/>
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A53" s="5">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -2347,14 +2537,19 @@
       <c r="D53" s="7">
         <v>8</v>
       </c>
-      <c r="J53" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="K53" t="s">
+      <c r="E53" s="13">
+        <v>79</v>
+      </c>
+      <c r="K53" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="L53" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="N53" s="12"/>
+      <c r="O53" s="12"/>
+    </row>
+    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A54" s="5">
         <f t="shared" si="0"/>
         <v>33</v>
@@ -2368,14 +2563,19 @@
       <c r="D54" s="7">
         <v>7.8</v>
       </c>
-      <c r="J54" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="K54" t="s">
+      <c r="E54" s="13">
+        <v>81</v>
+      </c>
+      <c r="K54" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="L54" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="N54" s="12"/>
+      <c r="O54" s="12"/>
+    </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A55" s="5">
         <f t="shared" si="0"/>
         <v>34</v>
@@ -2389,14 +2589,19 @@
       <c r="D55" s="7">
         <v>8</v>
       </c>
-      <c r="J55" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="K55" t="s">
+      <c r="E55" s="13">
+        <v>79</v>
+      </c>
+      <c r="K55" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="L55" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="N55" s="12"/>
+      <c r="O55" s="12"/>
+    </row>
+    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A56" s="5">
         <f t="shared" si="0"/>
         <v>35</v>
@@ -2410,14 +2615,19 @@
       <c r="D56" s="7">
         <v>7.3</v>
       </c>
-      <c r="J56" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="K56" t="s">
+      <c r="E56" s="13">
+        <v>86</v>
+      </c>
+      <c r="K56" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="L56" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="N56" s="12"/>
+      <c r="O56" s="12"/>
+    </row>
+    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A57" s="5">
         <f t="shared" si="0"/>
         <v>36</v>
@@ -2431,14 +2641,19 @@
       <c r="D57" s="7">
         <v>4</v>
       </c>
-      <c r="J57" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="K57" t="s">
+      <c r="E57" s="13">
+        <v>158</v>
+      </c>
+      <c r="K57" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="L57" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="N57" s="12"/>
+      <c r="O57" s="12"/>
+    </row>
+    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A58" s="5">
         <f t="shared" si="0"/>
         <v>37</v>
@@ -2452,14 +2667,19 @@
       <c r="D58" s="7">
         <v>7.3</v>
       </c>
-      <c r="J58" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="K58" t="s">
+      <c r="E58" s="13">
+        <v>86</v>
+      </c>
+      <c r="K58" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="L58" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="N58" s="12"/>
+      <c r="O58" s="12"/>
+    </row>
+    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A59" s="5">
         <f t="shared" si="0"/>
         <v>38</v>
@@ -2473,14 +2693,19 @@
       <c r="D59" s="7">
         <v>8</v>
       </c>
-      <c r="J59" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="K59" t="s">
+      <c r="E59" s="13">
+        <v>79</v>
+      </c>
+      <c r="K59" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="L59" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="N59" s="12"/>
+      <c r="O59" s="12"/>
+    </row>
+    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A60" s="5">
         <f t="shared" si="0"/>
         <v>39</v>
@@ -2494,14 +2719,19 @@
       <c r="D60" s="7">
         <v>4</v>
       </c>
-      <c r="J60" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="K60" t="s">
+      <c r="E60" s="13">
+        <v>158</v>
+      </c>
+      <c r="K60" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="L60" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="N60" s="12"/>
+      <c r="O60" s="12"/>
+    </row>
+    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A61" s="5">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -2515,14 +2745,19 @@
       <c r="D61" s="7">
         <v>10.3</v>
       </c>
-      <c r="J61" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="K61" t="s">
+      <c r="E61" s="13">
+        <v>61</v>
+      </c>
+      <c r="K61" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="L61" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="N61" s="12"/>
+      <c r="O61" s="12"/>
+    </row>
+    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A62" s="5">
         <f t="shared" si="0"/>
         <v>41</v>
@@ -2534,18 +2769,20 @@
         <v>82</v>
       </c>
       <c r="D62" s="7"/>
+      <c r="E62" s="7"/>
     </row>
   </sheetData>
-  <sortState ref="A21:G33">
-    <sortCondition ref="F21:F33"/>
+  <sortState ref="A21:H33">
+    <sortCondition ref="G21:G33"/>
   </sortState>
-  <mergeCells count="6">
+  <mergeCells count="7">
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="G1:K1"/>
+    <mergeCell ref="D1:D2"/>
     <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:J1"/>
-    <mergeCell ref="D1:D2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>